<commit_message>
Added the standard curve R2 values, slopes, and intercepts. These data will be used to make a table of R2 values, but also, a table of slopes and intercepts so that we can calculate the degree of interference that might be possible, like in Dirk's webinar.
</commit_message>
<xml_diff>
--- a/01_input/standard_curve_fits.xlsx
+++ b/01_input/standard_curve_fits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben.colman\Documents\Repositories\as_se_app_note\01_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B506B2D-AB81-4691-A035-BD5F4F058748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47CD384-8F57-4A4D-924D-371F96127A56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="20640" windowHeight="13200" xr2:uid="{5C84E667-ECF7-4528-AD43-1E99214E75B7}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{5C84E667-ECF7-4528-AD43-1E99214E75B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="27">
   <si>
     <t>Isotope</t>
   </si>
@@ -89,9 +89,6 @@
     <t>Unsure</t>
   </si>
   <si>
-    <t>Best fit?</t>
-  </si>
-  <si>
     <t>Really bad</t>
   </si>
   <si>
@@ -117,14 +114,25 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>Notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -155,7 +163,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,17 +480,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51CA7967-7DAA-407A-A77C-E97A9E0733F0}">
   <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46:H46"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="12.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -508,10 +516,10 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>74</v>
       </c>
@@ -537,7 +545,7 @@
         <v>0.99802999999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>75</v>
       </c>
@@ -563,7 +571,7 @@
         <v>0.99967099999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>76</v>
       </c>
@@ -589,7 +597,7 @@
         <v>0.99874300000000005</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>77</v>
       </c>
@@ -618,7 +626,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>78</v>
       </c>
@@ -644,7 +652,7 @@
         <v>0.99932799999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>80</v>
       </c>
@@ -670,10 +678,10 @@
         <v>0.86077999999999999</v>
       </c>
       <c r="I7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>82</v>
       </c>
@@ -699,7 +707,7 @@
         <v>0.99853000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>74</v>
       </c>
@@ -725,7 +733,7 @@
         <v>0.99885999999999997</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>75</v>
       </c>
@@ -751,10 +759,10 @@
         <v>0.99978500000000003</v>
       </c>
       <c r="I10" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>76</v>
       </c>
@@ -780,7 +788,7 @@
         <v>0.99933799999999995</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>77</v>
       </c>
@@ -806,10 +814,10 @@
         <v>0.99267700000000003</v>
       </c>
       <c r="I12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>78</v>
       </c>
@@ -835,7 +843,7 @@
         <v>0.99235200000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>80</v>
       </c>
@@ -861,7 +869,7 @@
         <v>0.99978500000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>82</v>
       </c>
@@ -883,11 +891,11 @@
       <c r="G15" s="1">
         <v>-5.9711700000000001E-7</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15">
         <v>0.99844500000000003</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>74</v>
       </c>
@@ -909,11 +917,11 @@
       <c r="G16" s="1">
         <v>-8.5671199999999994E-6</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16">
         <v>0.99990699999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>74</v>
       </c>
@@ -935,11 +943,11 @@
       <c r="G17" s="1">
         <v>-1.03409E-5</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17">
         <v>0.99973900000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>75</v>
       </c>
@@ -961,11 +969,11 @@
       <c r="G18" s="1">
         <v>9.9131100000000007E-6</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18">
         <v>0.99988600000000005</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>75</v>
       </c>
@@ -991,7 +999,7 @@
         <v>0.99975899999999995</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>76</v>
       </c>
@@ -1017,7 +1025,7 @@
         <v>0.99543800000000005</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>76</v>
       </c>
@@ -1043,10 +1051,10 @@
         <v>0.99739</v>
       </c>
       <c r="I21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>77</v>
       </c>
@@ -1072,7 +1080,7 @@
         <v>0.99537399999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>77</v>
       </c>
@@ -1098,7 +1106,7 @@
         <v>0.99715500000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>78</v>
       </c>
@@ -1124,7 +1132,7 @@
         <v>0.99921599999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>78</v>
       </c>
@@ -1150,7 +1158,7 @@
         <v>0.99898100000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>80</v>
       </c>
@@ -1176,7 +1184,7 @@
         <v>0.99987099999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>80</v>
       </c>
@@ -1202,7 +1210,7 @@
         <v>0.99975000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>82</v>
       </c>
@@ -1228,7 +1236,7 @@
         <v>0.99541900000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>82</v>
       </c>
@@ -1254,7 +1262,7 @@
         <v>0.99907999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>74</v>
       </c>
@@ -1262,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D30" t="s">
         <v>14</v>
@@ -1276,11 +1284,11 @@
       <c r="G30" s="1">
         <v>-2.7001900000000001E-6</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30">
         <v>0.998556</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>75</v>
       </c>
@@ -1288,7 +1296,7 @@
         <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D31" t="s">
         <v>13</v>
@@ -1306,7 +1314,7 @@
         <v>0.999973</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>76</v>
       </c>
@@ -1314,7 +1322,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D32" t="s">
         <v>13</v>
@@ -1328,11 +1336,11 @@
       <c r="G32" s="1">
         <v>-5.2472899999999997E-5</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32">
         <v>0.99983200000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>77</v>
       </c>
@@ -1340,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D33" t="s">
         <v>14</v>
@@ -1358,7 +1366,7 @@
         <v>0.99968999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>78</v>
       </c>
@@ -1366,7 +1374,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D34" t="s">
         <v>14</v>
@@ -1384,7 +1392,7 @@
         <v>0.99682899999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>80</v>
       </c>
@@ -1392,7 +1400,7 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -1410,7 +1418,7 @@
         <v>0.99961100000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>82</v>
       </c>
@@ -1418,7 +1426,7 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -1436,7 +1444,7 @@
         <v>0.998305</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>74</v>
       </c>
@@ -1444,7 +1452,7 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D37" t="s">
         <v>13</v>
@@ -1462,7 +1470,7 @@
         <v>0.99985800000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>75</v>
       </c>
@@ -1470,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D38" t="s">
         <v>14</v>
@@ -1488,10 +1496,10 @@
         <v>0.99972300000000003</v>
       </c>
       <c r="I38" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>76</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D39" t="s">
         <v>14</v>
@@ -1517,7 +1525,7 @@
         <v>0.99814400000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>77</v>
       </c>
@@ -1525,7 +1533,7 @@
         <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" t="s">
         <v>14</v>
@@ -1539,14 +1547,14 @@
       <c r="G40" s="1">
         <v>-4.3835000000000003E-5</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="2">
         <v>0.985294</v>
       </c>
       <c r="I40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>78</v>
       </c>
@@ -1554,7 +1562,7 @@
         <v>3</v>
       </c>
       <c r="C41" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" t="s">
         <v>14</v>
@@ -1572,7 +1580,7 @@
         <v>0.99972799999999995</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>80</v>
       </c>
@@ -1580,7 +1588,7 @@
         <v>3</v>
       </c>
       <c r="C42" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D42" t="s">
         <v>13</v>
@@ -1598,10 +1606,10 @@
         <v>0.99994899999999998</v>
       </c>
       <c r="I42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>82</v>
       </c>
@@ -1609,7 +1617,7 @@
         <v>3</v>
       </c>
       <c r="C43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D43" t="s">
         <v>14</v>
@@ -1627,7 +1635,7 @@
         <v>0.99350099999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>74</v>
       </c>
@@ -1635,7 +1643,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D44" t="s">
         <v>13</v>
@@ -1653,7 +1661,7 @@
         <v>0.99914000000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>75</v>
       </c>
@@ -1661,7 +1669,7 @@
         <v>4</v>
       </c>
       <c r="C45" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45" t="s">
         <v>14</v>
@@ -1679,7 +1687,7 @@
         <v>0.99964900000000001</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>76</v>
       </c>
@@ -1687,7 +1695,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D46" t="s">
         <v>13</v>
@@ -1705,7 +1713,7 @@
         <v>0.99627600000000005</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>77</v>
       </c>
@@ -1713,7 +1721,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D47" t="s">
         <v>14</v>
@@ -1731,7 +1739,7 @@
         <v>0.99757300000000004</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48">
         <v>78</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D48" t="s">
         <v>13</v>
@@ -1757,7 +1765,7 @@
         <v>0.99967600000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A49">
         <v>80</v>
       </c>
@@ -1765,25 +1773,25 @@
         <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G49" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H49" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>82</v>
       </c>
@@ -1791,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D50" t="s">
         <v>14</v>

</xml_diff>